<commit_message>
Commiting the new changes
</commit_message>
<xml_diff>
--- a/hybridFramework/src/test/resources/ExcelSheet/testDataHybrid.xlsx
+++ b/hybridFramework/src/test/resources/ExcelSheet/testDataHybrid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6910"/>
+    <workbookView windowWidth="19200" windowHeight="6910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="goibibo_Config" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Sl_no</t>
   </si>
@@ -29,19 +29,25 @@
     <t>1</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>searchHotelAndLogHotelName_TC01</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>searchHotelAndVerifyHotelDetail_TC02</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>searchHotelAndLogHotelName_TC01</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>searchHotelAndLogHotelName_TC02</t>
-  </si>
-  <si>
-    <t>searchHotelAndLogHotelName_TC03</t>
+    <t>searchHotelAndApplyFilter_TC03</t>
   </si>
   <si>
     <t>TestCaseID</t>
@@ -770,7 +776,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -779,9 +785,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,8 +1113,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1124,7 +1134,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1134,20 +1144,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1161,8 +1177,8 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1174,16 +1190,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1191,17 +1207,45 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="8"/>
+      <c r="C6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Pushing the new test case
</commit_message>
<xml_diff>
--- a/hybridFramework/src/test/resources/ExcelSheet/testDataHybrid.xlsx
+++ b/hybridFramework/src/test/resources/ExcelSheet/testDataHybrid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6910" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6910"/>
   </bookViews>
   <sheets>
     <sheet name="goibibo_Config" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Sl_no</t>
   </si>
@@ -29,25 +29,31 @@
     <t>1</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>searchHotelAndLogHotelName_TC01</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>searchHotelAndLogHotelName_TC01</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>searchHotelAndVerifyHotelDetail_TC02</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>searchHotelAndApplyFilter_TC03</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>searchHotelAndVerifyBooking_TC04</t>
   </si>
   <si>
     <t>TestCaseID</t>
@@ -1111,13 +1117,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="34.9090909090909" customWidth="1"/>
   </cols>
@@ -1149,21 +1155,32 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1177,8 +1194,8 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1190,16 +1207,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1207,27 +1224,27 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1235,13 +1252,27 @@
         <v>10</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="3:3">

</xml_diff>